<commit_message>
ajout des logs + info parametre
</commit_message>
<xml_diff>
--- a/parametre/Mercredi.xlsx
+++ b/parametre/Mercredi.xlsx
@@ -451,7 +451,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:M50"/>
+  <dimension ref="A3:M51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1412,7 +1412,26 @@
       <c r="M49" s="1" t="n"/>
     </row>
     <row r="50">
-      <c r="A50" t="inlineStr">
+      <c r="A50" s="3" t="inlineStr">
+        <is>
+          <t>FGHFG</t>
+        </is>
+      </c>
+      <c r="B50" s="3" t="n"/>
+      <c r="C50" s="3" t="n"/>
+      <c r="D50" s="3" t="n"/>
+      <c r="E50" s="3" t="n"/>
+      <c r="F50" s="3" t="n"/>
+      <c r="G50" s="3" t="n"/>
+      <c r="H50" s="3" t="n"/>
+      <c r="I50" s="3" t="n"/>
+      <c r="J50" s="3" t="n"/>
+      <c r="K50" s="3" t="n"/>
+      <c r="L50" s="3" t="n"/>
+      <c r="M50" s="3" t="n"/>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
         <is>
           <t>theme</t>
         </is>

</xml_diff>